<commit_message>
changed the layout of the page and also changed the active and inactive pages
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/ChefData.xlsx
+++ b/Group14-A2/src/main/java/User/ChefData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FDB4DE-AD12-4957-8B5F-F58F216DC823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103C4049-DD28-423E-BABD-AC3799130B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>User ID</t>
   </si>
@@ -53,13 +53,15 @@
   </si>
   <si>
     <t>Chef</t>
+  </si>
+  <si>
+    <t>Active Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,25 +407,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:XFD2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.93359375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7421875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.5859375" collapsed="true"/>
-    <col min="6" max="6" width="9.98828125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="13.984375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="11.375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,10 +450,13 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>5.0</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -462,17 +467,20 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="n">
-        <v>2.0</v>
+      <c r="E2">
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>20.0</v>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed the staff edit section and the whole manager control section
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/ChefData.xlsx
+++ b/Group14-A2/src/main/java/User/ChefData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
@@ -62,6 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,14 +416,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -464,8 +465,8 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2" t="n">
+        <v>20.0</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -473,14 +474,14 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="n">
+        <v>16.0</v>
       </c>
       <c r="H2">
         <v>20</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with the excel sheet
</commit_message>
<xml_diff>
--- a/Group14-A2/src/main/java/User/ChefData.xlsx
+++ b/Group14-A2/src/main/java/User/ChefData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\javafx-restaurant-app\Group14-A2\src\main\java\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103C4049-DD28-423E-BABD-AC3799130B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C69A3-2230-417B-9AD0-B20D5D090B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>User ID</t>
   </si>
@@ -56,13 +56,15 @@
   </si>
   <si>
     <t>Active Status</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,9 +114,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +154,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -258,7 +260,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,7 +402,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,23 +412,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
@@ -465,8 +467,8 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="n">
-        <v>20.0</v>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -474,8 +476,8 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="n">
-        <v>16.0</v>
+      <c r="G2">
+        <v>16</v>
       </c>
       <c r="H2">
         <v>20</v>

</xml_diff>